<commit_message>
Revisione Consegna Finale WBS
</commit_message>
<xml_diff>
--- a/Documenti/Scheduling e Cost/GreenLeaf Schedule.xlsx
+++ b/Documenti/Scheduling e Cost/GreenLeaf Schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/angeloafeltra/Documenti/GPS/Green-Leaf/Documenti/Scheduling e Cost/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Documents\Green-Leaf\Documenti\Scheduling e Cost\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A98BF8-8730-F94C-9527-83355877A227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A6F997F-4D1B-40FE-BA9D-0C026C2C3A71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabella_Attività" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="134">
   <si>
     <t>WBS</t>
   </si>
@@ -416,6 +416,15 @@
   </si>
   <si>
     <t>3g</t>
+  </si>
+  <si>
+    <t>1.9</t>
+  </si>
+  <si>
+    <t>Consegna Finale</t>
+  </si>
+  <si>
+    <t>2;14;21;25</t>
   </si>
 </sst>
 </file>
@@ -859,23 +868,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="159" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="36.33203125" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" customWidth="1"/>
-    <col min="5" max="6" width="19.5" customWidth="1"/>
+    <col min="3" max="3" width="10.1328125" customWidth="1"/>
+    <col min="4" max="4" width="11.1328125" customWidth="1"/>
+    <col min="5" max="6" width="19.46484375" customWidth="1"/>
     <col min="7" max="7" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -898,7 +907,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
@@ -915,11 +924,11 @@
         <v>44865</v>
       </c>
       <c r="F2" s="7">
-        <v>44952</v>
+        <v>44939</v>
       </c>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -940,7 +949,7 @@
       </c>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
         <v>15</v>
       </c>
@@ -961,7 +970,7 @@
       </c>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
@@ -982,7 +991,7 @@
       </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
@@ -1003,7 +1012,7 @@
       </c>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
@@ -1024,7 +1033,7 @@
       </c>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>31</v>
       </c>
@@ -1045,7 +1054,7 @@
       </c>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A9" s="5" t="s">
         <v>33</v>
       </c>
@@ -1068,7 +1077,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
         <v>36</v>
       </c>
@@ -1089,7 +1098,7 @@
       </c>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>39</v>
       </c>
@@ -1110,7 +1119,7 @@
       </c>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>42</v>
       </c>
@@ -1131,7 +1140,7 @@
       </c>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>45</v>
       </c>
@@ -1152,7 +1161,7 @@
       </c>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>47</v>
       </c>
@@ -1173,7 +1182,7 @@
       </c>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A15" s="5" t="s">
         <v>50</v>
       </c>
@@ -1196,7 +1205,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>54</v>
       </c>
@@ -1217,7 +1226,7 @@
       </c>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>57</v>
       </c>
@@ -1238,7 +1247,7 @@
       </c>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
         <v>59</v>
       </c>
@@ -1259,7 +1268,7 @@
       </c>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
         <v>61</v>
       </c>
@@ -1280,7 +1289,7 @@
       </c>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="2" t="s">
         <v>64</v>
       </c>
@@ -1301,7 +1310,7 @@
       </c>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
         <v>67</v>
       </c>
@@ -1322,7 +1331,7 @@
       </c>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A22" s="5" t="s">
         <v>69</v>
       </c>
@@ -1345,7 +1354,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="2" t="s">
         <v>72</v>
       </c>
@@ -1366,7 +1375,7 @@
       </c>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
         <v>74</v>
       </c>
@@ -1387,7 +1396,7 @@
       </c>
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A25" s="9" t="s">
         <v>77</v>
       </c>
@@ -1410,7 +1419,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A26" s="5" t="s">
         <v>82</v>
       </c>
@@ -1433,7 +1442,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="2" t="s">
         <v>86</v>
       </c>
@@ -1454,7 +1463,7 @@
       </c>
       <c r="G27" s="1"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="2" t="s">
         <v>89</v>
       </c>
@@ -1475,7 +1484,7 @@
       </c>
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="2" t="s">
         <v>91</v>
       </c>
@@ -1496,7 +1505,7 @@
       </c>
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A30" s="5" t="s">
         <v>93</v>
       </c>
@@ -1517,7 +1526,7 @@
       </c>
       <c r="G30" s="6"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="2" t="s">
         <v>96</v>
       </c>
@@ -1538,7 +1547,7 @@
       </c>
       <c r="G31" s="1"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="2" t="s">
         <v>98</v>
       </c>
@@ -1559,7 +1568,7 @@
       </c>
       <c r="G32" s="1"/>
     </row>
-    <row r="33" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A33" s="5" t="s">
         <v>101</v>
       </c>
@@ -1582,7 +1591,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" s="2" t="s">
         <v>105</v>
       </c>
@@ -1603,7 +1612,7 @@
       </c>
       <c r="G34" s="1"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="2" t="s">
         <v>108</v>
       </c>
@@ -1624,7 +1633,7 @@
       </c>
       <c r="G35" s="1"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="2" t="s">
         <v>110</v>
       </c>
@@ -1645,7 +1654,7 @@
       </c>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A37" s="5" t="s">
         <v>113</v>
       </c>
@@ -1668,7 +1677,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" s="2" t="s">
         <v>116</v>
       </c>
@@ -1689,7 +1698,7 @@
       </c>
       <c r="G38" s="1"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" s="2" t="s">
         <v>118</v>
       </c>
@@ -1710,7 +1719,7 @@
       </c>
       <c r="G39" s="1"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" s="2" t="s">
         <v>120</v>
       </c>
@@ -1731,7 +1740,7 @@
       </c>
       <c r="G40" s="1"/>
     </row>
-    <row r="41" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A41" s="5" t="s">
         <v>122</v>
       </c>
@@ -1752,7 +1761,7 @@
       </c>
       <c r="G41" s="6"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" s="2" t="s">
         <v>124</v>
       </c>
@@ -1773,7 +1782,7 @@
       </c>
       <c r="G42" s="1"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" s="2" t="s">
         <v>127</v>
       </c>
@@ -1793,6 +1802,29 @@
         <v>44966</v>
       </c>
       <c r="G43" s="1"/>
+    </row>
+    <row r="44" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A44" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E44" s="7">
+        <v>44970</v>
+      </c>
+      <c r="F44" s="7">
+        <v>44970</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>133</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>